<commit_message>
Updated 5 missing districts from MP: Singrauli, Tikamgarh, Ujjain, Umaria, Vidisha
</commit_message>
<xml_diff>
--- a/phase 2 release/districts extract/unique ph201d Indicators.xlsx
+++ b/phase 2 release/districts extract/unique ph201d Indicators.xlsx
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6">
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="7">
@@ -421,7 +421,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="8">
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="9">
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="11">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="12">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="13">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="15">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="17">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="18">
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="22">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="24">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="27">
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="30">
@@ -661,7 +661,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="32">
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35">
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="37">
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="39">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="40">
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="43">
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="44">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="47">
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="49">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="51">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="52">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="53">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="B54">
-        <v>695</v>
+        <v>700</v>
       </c>
     </row>
     <row r="55">
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="B57">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="58">
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="B58">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="59">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="B59">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="60">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="B60">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="61">
@@ -961,7 +961,7 @@
         </is>
       </c>
       <c r="B61">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="62">
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="B62">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="63">
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B64">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="65">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="B65">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="66">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="B66">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="67">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="B67">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="68">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="B69">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="70">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="B70">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71">
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="B71">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="72">
@@ -1071,7 +1071,7 @@
         </is>
       </c>
       <c r="B72">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="73">
@@ -1081,7 +1081,7 @@
         </is>
       </c>
       <c r="B73">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="74">
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="B74">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="75">
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="B75">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="76">
@@ -1111,7 +1111,7 @@
         </is>
       </c>
       <c r="B76">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="77">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="B78">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="79">
@@ -1141,7 +1141,7 @@
         </is>
       </c>
       <c r="B79">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="80">
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="B80">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="81">
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="B82">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="83">
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="B83">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="84">
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="B84">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="85">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="B85">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="86">
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="B86">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="87">
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="B87">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="88">
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="B88">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="89">
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="B89">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="90">
@@ -1251,7 +1251,7 @@
         </is>
       </c>
       <c r="B90">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="91">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="B91">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="92">
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="B92">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="93">
@@ -1281,7 +1281,7 @@
         </is>
       </c>
       <c r="B93">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="94">
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="B94">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="95">
@@ -1301,7 +1301,7 @@
         </is>
       </c>
       <c r="B95">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="96">
@@ -1311,7 +1311,7 @@
         </is>
       </c>
       <c r="B96">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="97">
@@ -1321,7 +1321,7 @@
         </is>
       </c>
       <c r="B97">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="98">
@@ -1341,7 +1341,7 @@
         </is>
       </c>
       <c r="B99">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="100">
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="B100">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="101">
@@ -1361,7 +1361,7 @@
         </is>
       </c>
       <c r="B101">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="102">
@@ -1371,7 +1371,7 @@
         </is>
       </c>
       <c r="B102">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="103">
@@ -1381,7 +1381,7 @@
         </is>
       </c>
       <c r="B103">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="104">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="B105">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="106">
@@ -1411,7 +1411,7 @@
         </is>
       </c>
       <c r="B106">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="107">
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="B108">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109">
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="B109">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="110">
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="B110">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="111">
@@ -1461,7 +1461,7 @@
         </is>
       </c>
       <c r="B111">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="112">
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="B112">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="113">
@@ -1481,7 +1481,7 @@
         </is>
       </c>
       <c r="B113">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="114">
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="B114">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="115">
@@ -1501,7 +1501,7 @@
         </is>
       </c>
       <c r="B115">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="116">
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="B116">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="117">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="B117">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="118">
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="B118">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="119">
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="B119">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="120">
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="B120">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="121">
@@ -1561,7 +1561,7 @@
         </is>
       </c>
       <c r="B121">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="122">
@@ -1571,7 +1571,7 @@
         </is>
       </c>
       <c r="B122">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="123">
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="B123">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="124">
@@ -1591,7 +1591,7 @@
         </is>
       </c>
       <c r="B124">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="125">
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="B125">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="126">
@@ -1611,7 +1611,7 @@
         </is>
       </c>
       <c r="B126">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="127">
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="B127">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="128">
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="B128">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="129">
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="B129">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="130">
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="B130">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="131">
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="B131">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="132">
@@ -1681,7 +1681,7 @@
         </is>
       </c>
       <c r="B133">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="134">
@@ -1691,7 +1691,7 @@
         </is>
       </c>
       <c r="B134">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="135">
@@ -1701,7 +1701,7 @@
         </is>
       </c>
       <c r="B135">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="136">
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="B137">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="138">
@@ -1741,7 +1741,7 @@
         </is>
       </c>
       <c r="B139">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="140">
@@ -1761,7 +1761,7 @@
         </is>
       </c>
       <c r="B141">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="142">
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="B143">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="144">

</xml_diff>